<commit_message>
close but no cigar:  1. I want the table(s) to take up a 1/3 of the page  2. both `Engine #10` and `2500 kW` are too much adjust right and not cell (based) adjusted...    1. Engine # - should be above the left column of the table     2. ukW - should be above Voltage
Signed-off-by: Ori Shadmon <oshadmon@gmail.com>
</commit_message>
<xml_diff>
--- a/demo/outputs/power_monitoring_report2.xlsx
+++ b/demo/outputs/power_monitoring_report2.xlsx
@@ -619,7 +619,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>12/16/2025 14:58:53</t>
+          <t>12/16/2025 16:04:57</t>
         </is>
       </c>
     </row>
@@ -638,16 +638,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t>Engine #10</t>
-        </is>
-      </c>
-      <c r="I5" s="5" t="inlineStr">
-        <is>
-          <t>3000kW</t>
-        </is>
-      </c>
+      <c r="B5" s="4" t="inlineStr"/>
+      <c r="I5" s="5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="6" t="n"/>

</xml_diff>